<commit_message>
Add xpaths for sub account
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GCEC-GIT\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FBE3D3-E15C-4C38-981E-3B616C689454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7EDA25-49BC-4D20-8946-96AFE8C912D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="112">
   <si>
     <t xml:space="preserve">ElementID </t>
   </si>
@@ -218,13 +218,151 @@
   </si>
   <si>
     <t>Geo_sb_delete_btn</t>
+  </si>
+  <si>
+    <t>settings_Tab</t>
+  </si>
+  <si>
+    <t>//div[contains(text(),'Settings')]</t>
+  </si>
+  <si>
+    <t>//a[normalize-space()='Sub Account']</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Add Sub Account')]//parent::button</t>
+  </si>
+  <si>
+    <t>Geofencing</t>
+  </si>
+  <si>
+    <t>Sub Account</t>
+  </si>
+  <si>
+    <t>sc_companyName</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Company Name')]//parent::div//parent::div//child::input</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Registration Code')]//parent::div//parent::div//child::input</t>
+  </si>
+  <si>
+    <t>sc_regCode</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Company Number')]//parent::div//parent::div//child::input</t>
+  </si>
+  <si>
+    <t>sc_companyNum</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Tax Number')]//parent::div//parent::div//child::input</t>
+  </si>
+  <si>
+    <t>sc_taxNum</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Email')]//parent::div//parent::div//child::input</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Phone Number')]//parent::div//parent::div//child::input</t>
+  </si>
+  <si>
+    <t>sc_phoneNum</t>
+  </si>
+  <si>
+    <t>sc_whatsappNum</t>
+  </si>
+  <si>
+    <t>sc_email</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Country')]//parent::div//parent::div//child::div//child::button</t>
+  </si>
+  <si>
+    <t>sc_country</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'WhatsApp Number')]//parent::div//parent::div//child::input</t>
+  </si>
+  <si>
+    <t>sc_state</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'State/Region')]//parent::div//parent::div//child::div//child::button</t>
+  </si>
+  <si>
+    <t>subAccount_Tab</t>
+  </si>
+  <si>
+    <t>//button[@type='submit']//span[contains(text(),'Add Sub Account')]</t>
+  </si>
+  <si>
+    <t>scf_AddBtn</t>
+  </si>
+  <si>
+    <t>sct_AddBtn</t>
+  </si>
+  <si>
+    <t>scp_firstName</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'First Name')]//parent::div//parent::div//child::input</t>
+  </si>
+  <si>
+    <t>scp_lastName</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Last Name')]//parent::div//parent::div//child::input</t>
+  </si>
+  <si>
+    <t>scp_password</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Password')]//parent::div//parent::div//child::input</t>
+  </si>
+  <si>
+    <t>scp_confPassword</t>
+  </si>
+  <si>
+    <t>(//span[contains(text(),'Password')]//parent::div//parent::div//child::input)[2]</t>
+  </si>
+  <si>
+    <t>scp_email</t>
+  </si>
+  <si>
+    <t>scp_phoneNum</t>
+  </si>
+  <si>
+    <t>scp_whatsappNum</t>
+  </si>
+  <si>
+    <t>scp_country</t>
+  </si>
+  <si>
+    <t>scp_state</t>
+  </si>
+  <si>
+    <t>(//span[contains(text(),'Email')]//parent::div//parent::div//child::input)[2]</t>
+  </si>
+  <si>
+    <t>(//span[contains(text(),'Phone Number')]//parent::div//parent::div//child::input)[2]</t>
+  </si>
+  <si>
+    <t>(//span[contains(text(),'WhatsApp Number')]//parent::div//parent::div//child::input)[2]</t>
+  </si>
+  <si>
+    <t>(//span[contains(text(),'Country')]//parent::div//parent::div//child::div//child::button)[2]</t>
+  </si>
+  <si>
+    <t>(//span[contains(text(),'State/Region')]//parent::div//parent::div//child::div//child::button)[2]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -232,13 +370,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -253,10 +429,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:C25"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,7 +784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -648,40 +836,40 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
+    <row r="9" spans="1:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -689,10 +877,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -700,50 +888,50 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
+    <row r="15" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -751,10 +939,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -762,10 +950,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -773,10 +961,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -784,10 +972,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -795,10 +983,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -806,10 +994,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -817,10 +1005,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -828,50 +1016,50 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
+    <row r="27" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -879,10 +1067,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -890,10 +1078,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -901,10 +1089,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -912,10 +1100,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -923,10 +1111,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -934,10 +1122,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
@@ -945,21 +1133,271 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>65</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>42</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>105</v>
+      </c>
+      <c r="B57" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A38:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement Sub account search
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GCEC-GIT\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60A5EDF-FB52-4B77-BE46-F5072EFC6FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEA712E-7BA3-4EB4-A357-A767C4C57FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="169">
   <si>
     <t xml:space="preserve">ElementID </t>
   </si>
@@ -46,9 +46,6 @@
     <t>Toast_message</t>
   </si>
   <si>
-    <t>//p[@class='mt-1 text-sm false text-[#03781D] false']</t>
-  </si>
-  <si>
     <t>settings_Icon</t>
   </si>
   <si>
@@ -515,6 +512,21 @@
   </si>
   <si>
     <t>//*[@id="root"]/div[1]/main/div[1]/div[2]/div/div[2]/button[2]/span</t>
+  </si>
+  <si>
+    <t>sct_searchBar</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Search Sub Account']</t>
+  </si>
+  <si>
+    <t>sct_firstRowEmail</t>
+  </si>
+  <si>
+    <t>(//div[@class='min-w-max']//child::div//child::span)[3]</t>
+  </si>
+  <si>
+    <t>//*[@id="_rht_toaster"]/div/div/div[1]/div/div[2]/p[2]</t>
   </si>
 </sst>
 </file>
@@ -610,6 +622,17 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -625,17 +648,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -950,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,11 +987,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -997,7 +1009,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1005,10 +1017,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1016,10 +1028,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1027,10 +1039,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
         <v>66</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1038,28 +1050,28 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1067,10 +1079,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1078,10 +1090,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1089,10 +1101,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
         <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -1100,28 +1112,28 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
         <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -1129,10 +1141,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -1140,10 +1152,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
         <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -1151,10 +1163,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
         <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1162,10 +1174,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
         <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -1173,10 +1185,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -1184,10 +1196,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
         <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>38</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -1195,10 +1207,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
         <v>39</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -1206,10 +1218,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
         <v>41</v>
-      </c>
-      <c r="B24" t="s">
-        <v>42</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -1217,10 +1229,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
         <v>43</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -1228,28 +1240,28 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
         <v>45</v>
       </c>
-      <c r="B26" t="s">
-        <v>46</v>
-      </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="A27" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
         <v>47</v>
-      </c>
-      <c r="B28" t="s">
-        <v>48</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -1257,10 +1269,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" t="s">
         <v>49</v>
-      </c>
-      <c r="B29" t="s">
-        <v>50</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -1268,10 +1280,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
         <v>51</v>
-      </c>
-      <c r="B30" t="s">
-        <v>52</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -1279,10 +1291,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
         <v>53</v>
-      </c>
-      <c r="B31" t="s">
-        <v>54</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -1290,10 +1302,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
         <v>55</v>
-      </c>
-      <c r="B32" t="s">
-        <v>56</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -1301,10 +1313,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
         <v>57</v>
-      </c>
-      <c r="B33" t="s">
-        <v>58</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -1312,10 +1324,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s">
         <v>59</v>
-      </c>
-      <c r="B34" t="s">
-        <v>60</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
@@ -1323,10 +1335,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" t="s">
         <v>61</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
@@ -1334,10 +1346,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" t="s">
         <v>63</v>
-      </c>
-      <c r="B36" t="s">
-        <v>64</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
@@ -1345,28 +1357,28 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="A38" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
@@ -1374,10 +1386,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" t="s">
         <v>72</v>
-      </c>
-      <c r="B40" t="s">
-        <v>73</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
@@ -1385,10 +1397,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
@@ -1396,10 +1408,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -1407,10 +1419,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
@@ -1418,10 +1430,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
@@ -1429,10 +1441,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
@@ -1440,10 +1452,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
@@ -1451,10 +1463,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
@@ -1462,10 +1474,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" t="s">
         <v>88</v>
-      </c>
-      <c r="B48" t="s">
-        <v>89</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
@@ -1473,10 +1485,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" t="s">
         <v>94</v>
-      </c>
-      <c r="B50" t="s">
-        <v>95</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
@@ -1484,10 +1496,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" t="s">
         <v>96</v>
-      </c>
-      <c r="B51" t="s">
-        <v>97</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
@@ -1495,10 +1507,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
         <v>98</v>
-      </c>
-      <c r="B52" t="s">
-        <v>99</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
@@ -1506,10 +1518,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" t="s">
         <v>100</v>
-      </c>
-      <c r="B53" t="s">
-        <v>101</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
@@ -1517,10 +1529,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
@@ -1528,10 +1540,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
@@ -1539,10 +1551,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
@@ -1550,10 +1562,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
@@ -1561,10 +1573,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
@@ -1572,10 +1584,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" t="s">
         <v>112</v>
-      </c>
-      <c r="B60" t="s">
-        <v>113</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
@@ -1583,10 +1595,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" t="s">
         <v>116</v>
-      </c>
-      <c r="B61" t="s">
-        <v>117</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
@@ -1594,10 +1606,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" t="s">
         <v>114</v>
-      </c>
-      <c r="B62" t="s">
-        <v>115</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
@@ -1605,294 +1617,316 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="8" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>164</v>
+      </c>
+      <c r="B65" t="s">
+        <v>165</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>166</v>
+      </c>
+      <c r="B66" t="s">
+        <v>167</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="6" t="s">
+      <c r="B68" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="C68" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C65" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
+      <c r="B69" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="C69" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C66" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="6" t="s">
+      <c r="B70" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="C70" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C67" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="6" t="s">
+      <c r="B71" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="C71" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C68" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="6" t="s">
+      <c r="B72" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="C72" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="6" t="s">
+      <c r="B73" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="C73" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="6" t="s">
+      <c r="B74" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="C74" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C71" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="6" t="s">
+      <c r="B75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="C75" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C72" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="6" t="s">
+      <c r="B76" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="C76" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C73" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="6" t="s">
+      <c r="B77" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="C77" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C74" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="6" t="s">
+      <c r="B78" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="C78" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C75" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="6" t="s">
+      <c r="B79" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C76" s="6"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="6" t="s">
+      <c r="B80" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="C80" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C77" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="6" t="s">
+      <c r="B81" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="C81" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C78" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="6" t="s">
+      <c r="B82" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="C82" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C79" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A80" s="7" t="s">
+      <c r="B83" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="C83" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C80" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A81" s="7" t="s">
+      <c r="B84" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="C84" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C81" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="7" t="s">
+      <c r="B85" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="C85" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C82" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A83" s="7" t="s">
+      <c r="B86" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="C86" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C83" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="9" t="s">
+      <c r="B87" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="C87" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="4"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+    </row>
+    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="4"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+    </row>
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="4"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C84" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="9"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-    </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="9"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-    </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="9"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="10"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="6" t="s">
+      <c r="B91" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="C91" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C88" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="6" t="s">
+      <c r="B92" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="C92" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C89" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="6" t="s">
+      <c r="B93" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B90" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="C90" s="6" t="s">
+      <c r="C93" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="C87:C90"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A15:C15"/>

</xml_diff>